<commit_message>
changes in btz figures
</commit_message>
<xml_diff>
--- a/CAICE/VOCs/Compiled_Compound_info_CAICE_VOC_SOAfocus.xlsx
+++ b/CAICE/VOCs/Compiled_Compound_info_CAICE_VOC_SOAfocus.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CAICE\VOC\NIST_lib_source_images\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40bfbb23b172f72e/Desktop/R_projects/New_GCxGC_analysis/CAICE/VOCs/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_CADF7F017EA29EE0CB27B422FDF8256980943188" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BE75574-F2E1-4722-AEB9-7FC9D24328E2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -317,7 +328,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -628,21 +639,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="24.77734375" customWidth="1"/>
-    <col min="11" max="11" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="11.5234375" customWidth="1"/>
+    <col min="3" max="3" width="24.7890625" customWidth="1"/>
+    <col min="10" max="10" width="19.9453125" customWidth="1"/>
+    <col min="11" max="11" width="21.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +698,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>23</v>
       </c>
@@ -724,7 +736,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>29</v>
       </c>
@@ -759,7 +771,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>84</v>
       </c>
@@ -797,7 +809,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>86</v>
       </c>
@@ -832,7 +844,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>87</v>
       </c>
@@ -867,7 +879,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>90</v>
       </c>
@@ -902,7 +914,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>123</v>
       </c>
@@ -937,7 +949,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>165</v>
       </c>
@@ -972,7 +984,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>168</v>
       </c>
@@ -1010,7 +1022,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>175</v>
       </c>
@@ -1045,7 +1057,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>183</v>
       </c>
@@ -1080,7 +1092,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>185</v>
       </c>
@@ -1112,7 +1124,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>208</v>
       </c>
@@ -1144,7 +1156,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>237</v>
       </c>
@@ -1182,7 +1194,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>287</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>308</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>333</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>391</v>
       </c>
@@ -1325,7 +1337,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>393</v>
       </c>
@@ -1357,7 +1369,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>498</v>
       </c>
@@ -1392,7 +1404,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>834</v>
       </c>
@@ -1425,7 +1437,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:J405">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J405">
     <sortCondition ref="D2:D405"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>